<commit_message>
fix: Nuevos ajustes para reportes
</commit_message>
<xml_diff>
--- a/plan_anual.xlsx
+++ b/plan_anual.xlsx
@@ -4,34 +4,208 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="true"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VICERRECTORIA ACADEMICA" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+  <si>
+    <t>Plan de acción 2022 VICERRECTORIA ACADEMICA</t>
+  </si>
+  <si>
+    <t>Armonización PED</t>
+  </si>
+  <si>
+    <t>Lineamiento</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Estrategias</t>
+  </si>
+  <si>
+    <t>Armonización Plan Indicativo</t>
+  </si>
+  <si>
+    <t>Factores</t>
+  </si>
+  <si>
+    <t>Lineaminetos de acción</t>
+  </si>
+  <si>
+    <t>N°.</t>
+  </si>
+  <si>
+    <t>Ponderación de la actividad</t>
+  </si>
+  <si>
+    <t>Periodo de ejecución</t>
+  </si>
+  <si>
+    <t>Actividad</t>
+  </si>
+  <si>
+    <t>Tareas</t>
+  </si>
+  <si>
+    <t>Indicador</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Fórmula</t>
+  </si>
+  <si>
+    <t>Lineamiento Estrategico 1. Formar ciudadanos, profesionales, investigadores, creadores e innovadores, íntegros con pensamiento crítico y cultura democrática, en contextos diferenciados inter y multiculturales para la transformación de la sociedad.</t>
+  </si>
+  <si>
+    <t>Meta 1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Consolidación de una oferta académica flexible que articule todas las metodologías de enseñanza, los niveles y los campos de formación, permitiendo el aumento y fortalecimiento de la oferta existente, articulada con la educación básica, media y superior.</t>
+  </si>
+  <si>
+    <t>Nivel 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nivel 2 </t>
+  </si>
+  <si>
+    <t>descripcion nivel 3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Trimestre 1</t>
+  </si>
+  <si>
+    <t>Actvidad 1</t>
+  </si>
+  <si>
+    <t>Tarea 1</t>
+  </si>
+  <si>
+    <t>Indicador 1</t>
+  </si>
+  <si>
+    <t>Indicador 2</t>
+  </si>
+  <si>
+    <t>Lineamiento Estrategico 2. Establecer un diseño curricular dinámico y flexible que promueva el pluralismo y consolide una comunidad universitaria crítica-transformadora y en armonía ambiental.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definición de lineamientos curriculares institucionales con enfoque crítico-transformador que fomenten el dialogo de saberes y conocimientos, la integración curricular, la pertinencia social, la flexibilidad, la interdisciplinariedad, la investigación curricular, la innovación y el uso de metodologías pertinentes a los diversos contextos. </t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Trimestre 2</t>
+  </si>
+  <si>
+    <t>Actividad 2</t>
+  </si>
+  <si>
+    <t>Tarea 22</t>
+  </si>
+  <si>
+    <t>indicador</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>Lineamiento Estrategico 3. Integrar las funciones universitarias por medio de la investigación, creación, innovación para la ampliación del conocimiento como bien público y para la solución de problemas de la ciudad - región y de la sociedad en general.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definición y desarrollo de modelos de apropiación social del conocimiento, que posibiliten el intercambio y diálogo de saberes y conocimientos con los sectores sociales, productivos y culturales. </t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Trimestre 3</t>
+  </si>
+  <si>
+    <t>actividad3</t>
+  </si>
+  <si>
+    <t>tarea3</t>
+  </si>
+  <si>
+    <t>LINEAMIENTO 5. Consolidar y fortalecer la democracia participativa, la gobernanza y la gobernabilidad para la cohesión de la comunidad universitaria</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Trimestre 4</t>
+  </si>
+  <si>
+    <t>actividad 4</t>
+  </si>
+  <si>
+    <t>tarea4</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -39,12 +213,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,9 +512,416 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col customWidth="true" max="6" min="1" width="70"/>
+    <col customWidth="true" max="9" min="8" width="20"/>
+    <col customWidth="true" max="11" min="10" width="80"/>
+    <col customWidth="true" max="14" min="12" width="50"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="true">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" ht="20" customHeight="true">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" ht="20" customHeight="true">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" ht="70" customHeight="true">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" ht="70" customHeight="true">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" ht="70" customHeight="true">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" ht="70" customHeight="true">
+      <c r="A8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="3">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" ht="70" customHeight="true">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="3">
+        <v>40</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="B4:B4"/>
+    <mergeCell ref="A4:A4"/>
+    <mergeCell ref="A5:A5"/>
+    <mergeCell ref="B5:B5"/>
+    <mergeCell ref="C5:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+  </mergeCells>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Ajuste para plan anual por unidad
</commit_message>
<xml_diff>
--- a/plan_anual.xlsx
+++ b/plan_anual.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="VICERRECTORIA ACADEMICA" sheetId="2" r:id="rId4"/>
+    <sheet name="Identificaciones" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Plan de acción 2022 VICERRECTORIA ACADEMICA</t>
   </si>
@@ -159,13 +160,157 @@
   </si>
   <si>
     <t>tarea4</t>
+  </si>
+  <si>
+    <t>Necesidades Presupuestales</t>
+  </si>
+  <si>
+    <t>Identificación de recursos:</t>
+  </si>
+  <si>
+    <t>Código del rubro</t>
+  </si>
+  <si>
+    <t>Nombre del rubro</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Descripción del bien y/o servicio</t>
+  </si>
+  <si>
+    <t>Actividades</t>
+  </si>
+  <si>
+    <t>3-01-002-02-02-08-0004-12</t>
+  </si>
+  <si>
+    <t>Servicios de telefonía fija (acceso)</t>
+  </si>
+  <si>
+    <t>$23,334,444.00</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1, 3</t>
+  </si>
+  <si>
+    <t>3-01-002-02-02-10-0003-00</t>
+  </si>
+  <si>
+    <t>Viáticos y gastos de viaje - Organizaciones Sindicales</t>
+  </si>
+  <si>
+    <t>$65,555.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4, 1</t>
+  </si>
+  <si>
+    <t>3-01-002-02-02-10-0002-01</t>
+  </si>
+  <si>
+    <t>VIÁTICOS Y GASTOS DE VIAJE - UAA</t>
+  </si>
+  <si>
+    <t>$233,333.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4, 2</t>
+  </si>
+  <si>
+    <t>Identificación de contratistas:</t>
+  </si>
+  <si>
+    <t>Descripción de la necesidad</t>
+  </si>
+  <si>
+    <t>Perfil</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>$17,878,700.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2</t>
+  </si>
+  <si>
+    <t>$2,429,171.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>$20,307,871.00</t>
+  </si>
+  <si>
+    <t>Identificación recurso docente:</t>
+  </si>
+  <si>
+    <t>Prima de servicios</t>
+  </si>
+  <si>
+    <t>$146,768.00</t>
+  </si>
+  <si>
+    <t>Prima de navidad</t>
+  </si>
+  <si>
+    <t>Prima de vacaciones</t>
+  </si>
+  <si>
+    <t>$82,192.00</t>
+  </si>
+  <si>
+    <t>Pensiones públicas</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>Salud</t>
+  </si>
+  <si>
+    <t>$168,377.00</t>
+  </si>
+  <si>
+    <t>Cesantias públicas</t>
+  </si>
+  <si>
+    <t>$55,236.00</t>
+  </si>
+  <si>
+    <t>Caja de compensación</t>
+  </si>
+  <si>
+    <t>$79,236.00</t>
+  </si>
+  <si>
+    <t>ARL</t>
+  </si>
+  <si>
+    <t>$10,324.00</t>
+  </si>
+  <si>
+    <t>ICBF</t>
+  </si>
+  <si>
+    <t>$59,440.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +329,20 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="26"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -232,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
@@ -242,6 +401,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,4 +1089,492 @@
     <mergeCell ref="K10:K11"/>
   </mergeCells>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col customWidth="true" max="6" min="1" width="30"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4"/>
+    <row r="5" ht="35" customHeight="true">
+      <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" ht="35" customHeight="true">
+      <c r="A6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" ht="35" customHeight="true">
+      <c r="A7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" ht="35" customHeight="true">
+      <c r="A8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11"/>
+    <row r="12" ht="35" customHeight="true">
+      <c r="A12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" ht="35" customHeight="true">
+      <c r="A13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="3">
+        <v>486</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" ht="35" customHeight="true">
+      <c r="A14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3">
+        <v>484</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" ht="35" customHeight="true">
+      <c r="A15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16"/>
+    <row r="17">
+      <c r="A17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18"/>
+    <row r="19" ht="35" customHeight="true">
+      <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" ht="35" customHeight="true">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" ht="35" customHeight="true">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" ht="35" customHeight="true">
+      <c r="A22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" ht="35" customHeight="true">
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" ht="35" customHeight="true">
+      <c r="A24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" ht="35" customHeight="true">
+      <c r="A25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" ht="35" customHeight="true">
+      <c r="A26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" ht="35" customHeight="true">
+      <c r="A27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" ht="35" customHeight="true">
+      <c r="A28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200">
+      <c r="A200" s="3"/>
+      <c r="B200" s="3"/>
+      <c r="C200" s="3"/>
+      <c r="D200" s="3"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:F4"/>
+    <mergeCell ref="A10:F11"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:F18"/>
+  </mergeCells>
+</worksheet>
 </file>
</xml_diff>